<commit_message>
new excel code generator pre final
first impl. of the layer framework
</commit_message>
<xml_diff>
--- a/frames_list.xlsx
+++ b/frames_list.xlsx
@@ -1,32 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcel\Desktop\WeatherFrame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelochsendorf/Desktop/WeatherFrame/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="3" r:id="rId1"/>
     <sheet name="RAIN ANIMATION" sheetId="1" r:id="rId2"/>
     <sheet name="COLOR PALETTE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -92,12 +95,27 @@
   </si>
   <si>
     <t>ANIMATION FRAMES</t>
+  </si>
+  <si>
+    <t>COLOR_STRUCT_NAME</t>
+  </si>
+  <si>
+    <t>COLOR_DESC</t>
+  </si>
+  <si>
+    <t>generated color struct name</t>
+  </si>
+  <si>
+    <t>color_struct_name</t>
+  </si>
+  <si>
+    <t>CD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -146,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,15 +196,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFF9522C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF68F442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -205,69 +241,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF68F442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF659CEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9522C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -281,9 +254,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -588,11 +558,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -604,21 +576,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ26"/>
+  <dimension ref="A1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.1640625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" style="3"/>
-    <col min="3" max="3" width="6.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.125" style="3"/>
+    <col min="1" max="1" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="3"/>
+    <col min="3" max="3" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="5.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -676,7 +648,7 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3">
         <v>0</v>
@@ -782,7 +754,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="3">
         <v>0</v>
@@ -888,7 +860,7 @@
       </c>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="3">
         <v>0</v>
@@ -994,7 +966,7 @@
       </c>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="3">
         <v>0</v>
@@ -1100,7 +1072,7 @@
       </c>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="3">
         <v>0</v>
@@ -1206,7 +1178,7 @@
       </c>
       <c r="AQ6" s="1"/>
     </row>
-    <row r="7" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="3">
         <v>0</v>
@@ -1312,7 +1284,7 @@
       </c>
       <c r="AQ7" s="1"/>
     </row>
-    <row r="8" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="3">
         <v>0</v>
@@ -1418,7 +1390,7 @@
       </c>
       <c r="AQ8" s="1"/>
     </row>
-    <row r="9" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>2</v>
@@ -1524,7 +1496,7 @@
       </c>
       <c r="AQ9" s="1"/>
     </row>
-    <row r="10" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1566,30 +1538,35 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
     </row>
-    <row r="12" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5">
+      <c r="E13" s="9">
         <v>4</v>
       </c>
       <c r="F13" s="5"/>
@@ -1600,12 +1577,12 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="str">
-        <f>"{"&amp;B2&amp;","&amp; C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;"}"</f>
-        <v>{0,2,0,0,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(B2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1615,26 +1592,26 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="N14" s="5" t="str">
-        <f>"{"&amp;M2&amp;","&amp; N2&amp;","&amp;O2&amp;","&amp;P2&amp;","&amp;Q2&amp;","&amp;R2&amp;","&amp;S2&amp;","&amp;T2&amp;"}"</f>
-        <v>{2,0,0,2,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(M2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Y14" s="5" t="str">
-        <f>"{"&amp;X2&amp;","&amp; Y2&amp;","&amp;Z2&amp;","&amp;AA2&amp;","&amp;AB2&amp;","&amp;AC2&amp;","&amp;AD2&amp;","&amp;AE2&amp;"}"</f>
-        <v>{0,0,0,0,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(X2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="AJ14" s="5" t="str">
-        <f>"{"&amp;AI2&amp;","&amp; AJ2&amp;","&amp;AK2&amp;","&amp;AL2&amp;","&amp;AM2&amp;","&amp;AN2&amp;","&amp;AO2&amp;","&amp;AP2&amp;"}"</f>
-        <v>{0,0,0,2,0,0,0,2}</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP2,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237)}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="str">
-        <f>"{"&amp;B3&amp;","&amp; C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;"}"</f>
-        <v>{0,2,0,0,2,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(B3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1644,25 +1621,25 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="N15" s="5" t="str">
-        <f t="shared" ref="N15:N21" si="0">"{"&amp;M3&amp;","&amp; N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;"}"</f>
-        <v>{2,2,0,2,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(M3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="O15" s="5"/>
       <c r="Y15" s="5" t="str">
-        <f t="shared" ref="Y15:Y21" si="1">"{"&amp;X3&amp;","&amp; Y3&amp;","&amp;Z3&amp;","&amp;AA3&amp;","&amp;AB3&amp;","&amp;AC3&amp;","&amp;AD3&amp;","&amp;AE3&amp;"}"</f>
-        <v>{2,0,0,2,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(X3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="AJ15" s="5" t="str">
-        <f t="shared" ref="AJ15:AJ21" si="2">"{"&amp;AI3&amp;","&amp; AJ3&amp;","&amp;AK3&amp;","&amp;AL3&amp;","&amp;AM3&amp;","&amp;AN3&amp;","&amp;AO3&amp;","&amp;AP3&amp;"}"</f>
-        <v>{0,0,0,2,0,0,0,0}</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP3,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="str">
-        <f>"{"&amp;B4&amp;","&amp; C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4&amp;"}"</f>
-        <v>{0,0,2,0,2,0,0,2}</v>
+        <f>"{"&amp; VLOOKUP(B4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1672,24 +1649,24 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,2,0,0,2,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(M4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="Y16" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{2,2,0,2,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(X4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="AJ16" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{2,0,0,0,0,0,0,0}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP4,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="str">
-        <f>"{"&amp;B5&amp;","&amp; C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;"}"</f>
-        <v>{0,0,2,0,0,2,0,2}</v>
+        <f>"{"&amp; VLOOKUP(B5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1699,24 +1676,24 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="N17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,0,2,0,2,0,0,2}</v>
+        <f>"{"&amp; VLOOKUP(M5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="Y17" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{0,2,0,0,2,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(X5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="AJ17" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{2,2,0,2,0,0,2,0}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP5,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="str">
-        <f>"{"&amp;B6&amp;","&amp; C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6&amp;"}"</f>
-        <v>{0,2,0,0,0,2,0,0}</v>
+        <f>"{"&amp; VLOOKUP(B6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1726,24 +1703,24 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="N18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,0,2,0,0,2,0,2}</v>
+        <f>"{"&amp; VLOOKUP(M6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="Y18" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{0,0,2,0,2,0,0,2}</v>
+        <f>"{"&amp; VLOOKUP(X6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="AJ18" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{0,2,0,2,2,0,2,0}</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP6,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="str">
-        <f>"{"&amp;B7&amp;","&amp; C7&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;"}"</f>
-        <v>{0,2,0,2,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(B7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1753,24 +1730,24 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="N19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,2,0,0,0,2,0,0}</v>
+        <f>"{"&amp; VLOOKUP(M7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="Y19" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{0,0,2,0,0,2,0,2}</v>
+        <f>"{"&amp; VLOOKUP(X7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)}</v>
       </c>
       <c r="AJ19" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{0,0,2,0,2,0,0,2}</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP7,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="str">
-        <f>"{"&amp;B8&amp;","&amp; C8&amp;","&amp;D8&amp;","&amp;E8&amp;","&amp;F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8&amp;"}"</f>
-        <v>{0,0,0,2,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(B8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1780,24 +1757,24 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="N20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>{0,2,0,2,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(M8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="Y20" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{0,2,0,0,0,2,0,0}</v>
+        <f>"{"&amp; VLOOKUP(X8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="AJ20" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{0,0,2,0,0,2,0,2}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP8,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="str">
-        <f>"{"&amp;B9&amp;","&amp; C9&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9&amp;"}"</f>
-        <v>{2,0,0,0,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(B9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(C9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(D9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(E9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(F9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(G9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(H9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(I9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1807,54 +1784,84 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="N21" s="5" t="str">
-        <f>"{"&amp;M9&amp;","&amp; N9&amp;","&amp;O9&amp;","&amp;P9&amp;","&amp;Q9&amp;","&amp;R9&amp;","&amp;S9&amp;","&amp;T9&amp;"}"</f>
-        <v>{0,0,0,2,0,0,2,0}</v>
+        <f>"{"&amp; VLOOKUP(M9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(N9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(O9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(P9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Q9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(R9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(S9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(T9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)}</v>
       </c>
       <c r="Y21" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{0,2,0,2,0,0,0,0}</v>
+        <f>"{"&amp; VLOOKUP(X9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(Y9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(Z9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AA9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AB9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AC9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AD9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AE9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)}</v>
       </c>
       <c r="AJ21" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>{0,2,0,0,0,2,0,0}</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f>"{"&amp; VLOOKUP(AI9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp; VLOOKUP(AJ9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AK9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AL9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AM9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AN9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AO9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;","&amp;VLOOKUP(AP9,'COLOR PALETTE'!$A$2:$G$6,7)&amp;"}"</f>
+        <v>{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="str">
-        <f xml:space="preserve"> "const animation_" &amp; E12 &amp; " [" &amp; E13 &amp;"][8][8] = {"</f>
-        <v>const animation_rain [4][8][8] = {</v>
+        <f xml:space="preserve"> "const frame_data [" &amp; E13 &amp;"][8][8] = {"</f>
+        <v>const frame_data [4][8][8] = {</v>
       </c>
       <c r="G24" s="8" t="str">
         <f xml:space="preserve"> "{"&amp; C14 &amp;","&amp;C15 &amp;","&amp;C16 &amp;","&amp;C17&amp;","&amp;C18 &amp;","&amp;C19 &amp;","&amp;C20 &amp;","&amp;C21 &amp;"," &amp;"},"</f>
-        <v>{{0,2,0,0,0,0,2,0},{0,2,0,0,2,0,2,0},{0,0,2,0,2,0,0,2},{0,0,2,0,0,2,0,2},{0,2,0,0,0,2,0,0},{0,2,0,2,0,0,0,0},{0,0,0,2,0,0,2,0},{2,0,0,0,0,0,2,0},},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>{{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="8" t="str">
         <f xml:space="preserve"> "{"&amp; N14 &amp;","&amp;N15 &amp;","&amp;N16 &amp;","&amp;N17&amp;","&amp;N18 &amp;","&amp;N19 &amp;","&amp;N20 &amp;","&amp;N21 &amp;"," &amp;"},"</f>
-        <v>{{2,0,0,2,0,0,0,0},{2,2,0,2,0,0,2,0},{0,2,0,0,2,0,2,0},{0,0,2,0,2,0,0,2},{0,0,2,0,0,2,0,2},{0,2,0,0,0,2,0,0},{0,2,0,2,0,0,0,0},{0,0,0,2,0,0,2,0},},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="8"/>
+        <v>{{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="8" t="str">
+        <f xml:space="preserve"> "{"&amp; Y14 &amp;","&amp;Y15 &amp;","&amp;Y16 &amp;","&amp;Y17&amp;","&amp;Y18 &amp;","&amp;Y19 &amp;","&amp;Y20 &amp;","&amp;Y21 &amp;"," &amp;"},"</f>
+        <v>{{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="8" t="str">
+        <f xml:space="preserve"> "{"&amp; AJ14 &amp;","&amp;AJ15 &amp;","&amp;AJ16 &amp;","&amp;AJ17&amp;","&amp;AJ18 &amp;","&amp;AJ19 &amp;","&amp;AJ20 &amp;","&amp;AJ21 &amp;"," &amp;"},"</f>
+        <v>{{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(0,0,0)},{CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(100,149,237)},{CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0),CD(0,0,0),CD(100,149,237),CD(0,0,0),CD(0,0,0)},},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="3" t="str">
+        <f xml:space="preserve"> "}"</f>
+        <v>}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="str">
+        <f xml:space="preserve"> "const std::string animation_name = " &amp; E12 &amp;";"</f>
+        <v>const std::string animation_name = rain;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="str">
+        <f>"const int"</f>
+        <v>const int</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:I9 M2:T9 X2:AE9 AI2:AP9">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I9 M2:T9 X2:AE9 AI2:AP9">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1865,19 +1872,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1896,8 +1904,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1916,8 +1927,12 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>$K$8 &amp; "(" &amp; D2 &amp; "," &amp; E2 &amp; "," &amp; F2 &amp; ")"</f>
+        <v>CD(0,0,0)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1936,8 +1951,12 @@
       <c r="F3">
         <v>255</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G6" si="0">$K$8 &amp; "(" &amp; D3 &amp; "," &amp; E3 &amp; "," &amp; F3 &amp; ")"</f>
+        <v>CD(255,255,255)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1956,8 +1975,12 @@
       <c r="F4">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>CD(100,149,237)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1976,8 +1999,12 @@
       <c r="F5">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>CD(249,82,44)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1996,6 +2023,25 @@
       <c r="F6">
         <v>66</v>
       </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>CD(104,244,66)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G8" s="11"/>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>